<commit_message>
scrollBox.html and withXLSX.js are latest
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coolf\Downloads\doing-something\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coolf\Downloads\trl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309D0248-EFD1-407E-BC07-8C27934EFBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04D4834-13FA-462A-BA6F-9EA47B68D079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5565" uniqueCount="2385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5568" uniqueCount="2385">
   <si>
     <t>Design of Next Generation Noise And Vibration Sensor Fusion Module</t>
   </si>
@@ -7617,8 +7617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H928"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
-      <selection activeCell="E220" sqref="E220"/>
+    <sheetView tabSelected="1" topLeftCell="A910" workbookViewId="0">
+      <selection activeCell="L928" sqref="L928"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13772,6 +13772,9 @@
       <c r="C237" t="s">
         <v>700</v>
       </c>
+      <c r="D237" t="s">
+        <v>2384</v>
+      </c>
       <c r="E237" t="s">
         <v>4</v>
       </c>
@@ -13947,6 +13950,12 @@
       </c>
       <c r="B244" t="s">
         <v>411</v>
+      </c>
+      <c r="C244" t="s">
+        <v>2384</v>
+      </c>
+      <c r="D244" t="s">
+        <v>2384</v>
       </c>
       <c r="E244" t="s">
         <v>15</v>

</xml_diff>